<commit_message>
H4 nagelezen voor een eerste keer
</commit_message>
<xml_diff>
--- a/Thesis - 2/Nodig/SystemTable.xlsx
+++ b/Thesis - 2/Nodig/SystemTable.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Persistentie</t>
   </si>
@@ -39,6 +39,9 @@
     <t>Query soort</t>
   </si>
   <si>
+    <t>Range</t>
+  </si>
+  <si>
     <t>Cassandra</t>
   </si>
   <si>
@@ -114,9 +117,6 @@
     <t>Master-Master</t>
   </si>
   <si>
-    <t>MasterSlave</t>
-  </si>
-  <si>
     <t>Nee</t>
   </si>
   <si>
@@ -132,7 +132,13 @@
     <t>Uitleggen van aanpassen</t>
   </si>
   <si>
-    <t>Scan</t>
+    <t>Mogelijk</t>
+  </si>
+  <si>
+    <t>Half</t>
+  </si>
+  <si>
+    <t>Snapshots</t>
   </si>
 </sst>
 </file>
@@ -521,19 +527,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +571,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +581,7 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -604,51 +611,51 @@
         <v>33</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>34</v>
@@ -656,31 +663,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -691,45 +698,51 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -743,14 +756,20 @@
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -758,78 +777,111 @@
         <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>